<commit_message>
print cross validation scores into Excel file
</commit_message>
<xml_diff>
--- a/results/feature_importance_to_performance_in_online.xlsx
+++ b/results/feature_importance_to_performance_in_online.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="feature_importance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="cv_scores" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -668,4 +669,70 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cross-validation R^2 scores</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.310646068017594</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.2424582917579408</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.4400098584980944</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.3365234053737414</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5022688053484423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>